<commit_message>
New sheet Branch 2
</commit_message>
<xml_diff>
--- a/VC Test Cases.xlsx
+++ b/VC Test Cases.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="VC Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="86">
   <si>
     <t>Test Iteration 1</t>
   </si>
@@ -329,6 +330,9 @@
   </si>
   <si>
     <t>More additions</t>
+  </si>
+  <si>
+    <t>Branch 2 added</t>
   </si>
 </sst>
 </file>
@@ -422,26 +426,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -834,139 +838,139 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="19"/>
+      <c r="A1" s="16"/>
+      <c r="B1" s="16"/>
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="21">
+      <c r="B6" s="18"/>
+      <c r="C6" s="19">
         <f ca="1">TODAY()</f>
         <v>42101</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="17"/>
+      <c r="B7" s="18"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="15"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="17"/>
+      <c r="B13" s="18"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="15">
         <v>20110137</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18" t="s">
+      <c r="B16" s="18"/>
+      <c r="C16" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
@@ -992,10 +996,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="15"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
@@ -1104,10 +1108,10 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="15"/>
+      <c r="B33" s="20"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
@@ -1161,10 +1165,10 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="15"/>
+      <c r="B41" s="20"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
@@ -1271,10 +1275,10 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B54" s="15"/>
+      <c r="B54" s="20"/>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
@@ -1392,6 +1396,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="A4:B5"/>
@@ -1404,13 +1415,6 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A41:B41"/>
   </mergeCells>
   <conditionalFormatting sqref="G17">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
@@ -1437,7 +1441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1461,4 +1465,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Testing deletion of line
</commit_message>
<xml_diff>
--- a/VC Test Cases.xlsx
+++ b/VC Test Cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="VC Test Cases" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="87">
   <si>
     <t>Test Iteration 1</t>
   </si>
@@ -333,6 +333,9 @@
   </si>
   <si>
     <t>Branch 2 added</t>
+  </si>
+  <si>
+    <t>Test deletion</t>
   </si>
 </sst>
 </file>
@@ -426,26 +429,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -823,7 +826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -838,139 +841,139 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="19"/>
+      <c r="A1" s="16"/>
+      <c r="B1" s="16"/>
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="21">
+      <c r="B6" s="18"/>
+      <c r="C6" s="19">
         <f ca="1">TODAY()</f>
         <v>42101</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="17"/>
+      <c r="B7" s="18"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="15"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="17"/>
+      <c r="B13" s="18"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="15">
         <v>20110137</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18" t="s">
+      <c r="B16" s="18"/>
+      <c r="C16" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
@@ -996,10 +999,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="15"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
@@ -1108,10 +1111,10 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="15"/>
+      <c r="B33" s="20"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
@@ -1165,10 +1168,10 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="15"/>
+      <c r="B41" s="20"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
@@ -1275,10 +1278,10 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B54" s="15"/>
+      <c r="B54" s="20"/>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
@@ -1396,6 +1399,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="A4:B5"/>
@@ -1408,13 +1418,6 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A41:B41"/>
   </mergeCells>
   <conditionalFormatting sqref="G17">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
@@ -1469,10 +1472,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2"/>
+  <dimension ref="B2:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,6 +1485,11 @@
         <v>85</v>
       </c>
     </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>